<commit_message>
add new trimmed mds and extracted data
</commit_message>
<xml_diff>
--- a/data/temp/character_count.xlsx
+++ b/data/temp/character_count.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Filename</t>
   </si>
@@ -22,34 +22,280 @@
     <t>Character Count</t>
   </si>
   <si>
+    <t>Estimated Tokens</t>
+  </si>
+  <si>
+    <t>28.md</t>
+  </si>
+  <si>
+    <t>79.md</t>
+  </si>
+  <si>
+    <t>5.md</t>
+  </si>
+  <si>
+    <t>69.md</t>
+  </si>
+  <si>
+    <t>38.md</t>
+  </si>
+  <si>
     <t>49.md</t>
   </si>
   <si>
+    <t>59.md</t>
+  </si>
+  <si>
+    <t>1.md</t>
+  </si>
+  <si>
+    <t>19.md</t>
+  </si>
+  <si>
     <t>48.md</t>
   </si>
   <si>
+    <t>58.md</t>
+  </si>
+  <si>
+    <t>29.md</t>
+  </si>
+  <si>
+    <t>78.md</t>
+  </si>
+  <si>
+    <t>101.md</t>
+  </si>
+  <si>
+    <t>4.md</t>
+  </si>
+  <si>
+    <t>68.md</t>
+  </si>
+  <si>
+    <t>39.md</t>
+  </si>
+  <si>
+    <t>47.md</t>
+  </si>
+  <si>
+    <t>16.md</t>
+  </si>
+  <si>
+    <t>80.md</t>
+  </si>
+  <si>
+    <t>22.md</t>
+  </si>
+  <si>
+    <t>73.md</t>
+  </si>
+  <si>
     <t>63.md</t>
   </si>
   <si>
+    <t>32.md</t>
+  </si>
+  <si>
+    <t>90.md</t>
+  </si>
+  <si>
+    <t>57.md</t>
+  </si>
+  <si>
+    <t>84.md</t>
+  </si>
+  <si>
+    <t>77.md</t>
+  </si>
+  <si>
+    <t>26.md</t>
+  </si>
+  <si>
+    <t>12.md</t>
+  </si>
+  <si>
+    <t>43.md</t>
+  </si>
+  <si>
+    <t>53.md</t>
+  </si>
+  <si>
+    <t>36.md</t>
+  </si>
+  <si>
+    <t>67.md</t>
+  </si>
+  <si>
+    <t>94.md</t>
+  </si>
+  <si>
+    <t>85.md</t>
+  </si>
+  <si>
     <t>76.md</t>
   </si>
   <si>
+    <t>13.md</t>
+  </si>
+  <si>
+    <t>42.md</t>
+  </si>
+  <si>
+    <t>52.md</t>
+  </si>
+  <si>
+    <t>37.md</t>
+  </si>
+  <si>
+    <t>66.md</t>
+  </si>
+  <si>
+    <t>95.md</t>
+  </si>
+  <si>
+    <t>46.md</t>
+  </si>
+  <si>
+    <t>17.md</t>
+  </si>
+  <si>
+    <t>81.md</t>
+  </si>
+  <si>
+    <t>23.md</t>
+  </si>
+  <si>
+    <t>72.md</t>
+  </si>
+  <si>
     <t>62.md</t>
   </si>
   <si>
+    <t>33.md</t>
+  </si>
+  <si>
+    <t>91.md</t>
+  </si>
+  <si>
+    <t>56.md</t>
+  </si>
+  <si>
+    <t>24.md</t>
+  </si>
+  <si>
     <t>75.md</t>
   </si>
   <si>
+    <t>86.md</t>
+  </si>
+  <si>
+    <t>41.md</t>
+  </si>
+  <si>
+    <t>10.md</t>
+  </si>
+  <si>
+    <t>51.md</t>
+  </si>
+  <si>
+    <t>9.md</t>
+  </si>
+  <si>
+    <t>65.md</t>
+  </si>
+  <si>
+    <t>34.md</t>
+  </si>
+  <si>
+    <t>14.md</t>
+  </si>
+  <si>
+    <t>45.md</t>
+  </si>
+  <si>
+    <t>20.md</t>
+  </si>
+  <si>
+    <t>82.md</t>
+  </si>
+  <si>
+    <t>30.md</t>
+  </si>
+  <si>
     <t>61.md</t>
   </si>
   <si>
+    <t>55.md</t>
+  </si>
+  <si>
+    <t>15.md</t>
+  </si>
+  <si>
+    <t>44.md</t>
+  </si>
+  <si>
+    <t>83.md</t>
+  </si>
+  <si>
+    <t>31.md</t>
+  </si>
+  <si>
     <t>60.md</t>
   </si>
   <si>
+    <t>54.md</t>
+  </si>
+  <si>
+    <t>25.md</t>
+  </si>
+  <si>
     <t>74.md</t>
   </si>
   <si>
+    <t>87.md</t>
+  </si>
+  <si>
+    <t>40.md</t>
+  </si>
+  <si>
+    <t>11.md</t>
+  </si>
+  <si>
+    <t>50.md</t>
+  </si>
+  <si>
+    <t>8.md</t>
+  </si>
+  <si>
+    <t>97.md</t>
+  </si>
+  <si>
+    <t>64.md</t>
+  </si>
+  <si>
+    <t>35.md</t>
+  </si>
+  <si>
+    <t>3.md</t>
+  </si>
+  <si>
+    <t>88.md</t>
+  </si>
+  <si>
+    <t>102.md</t>
+  </si>
+  <si>
+    <t>98.md</t>
+  </si>
+  <si>
     <t>89.md</t>
+  </si>
+  <si>
+    <t>6.md</t>
+  </si>
+  <si>
+    <t>2.md</t>
   </si>
 </sst>
 </file>
@@ -407,98 +653,1022 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
+        <v>93013</v>
+      </c>
+      <c r="C2">
+        <v>23253.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>472000</v>
+      </c>
+      <c r="C3">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>472000</v>
+      </c>
+      <c r="C4">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>75273</v>
+      </c>
+      <c r="C5">
+        <v>18818.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>472000</v>
+      </c>
+      <c r="C6">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
         <v>122004</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+      <c r="C7">
+        <v>30501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>63134</v>
+      </c>
+      <c r="C8">
+        <v>15783.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>183369</v>
+      </c>
+      <c r="C9">
+        <v>45842.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>79091</v>
+      </c>
+      <c r="C10">
+        <v>19772.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
         <v>45650</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1097448</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+      <c r="C11">
+        <v>11412.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>47220</v>
+      </c>
+      <c r="C12">
+        <v>11805</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>48707</v>
+      </c>
+      <c r="C13">
+        <v>12176.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>42369</v>
+      </c>
+      <c r="C14">
+        <v>10592.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>472000</v>
+      </c>
+      <c r="C15">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>70440</v>
+      </c>
+      <c r="C16">
+        <v>17610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>59621</v>
+      </c>
+      <c r="C17">
+        <v>14905.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>152929</v>
+      </c>
+      <c r="C18">
+        <v>38232.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>66009</v>
+      </c>
+      <c r="C19">
+        <v>16502.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>78501</v>
+      </c>
+      <c r="C20">
+        <v>19625.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>65382</v>
+      </c>
+      <c r="C21">
+        <v>16345.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>472000</v>
+      </c>
+      <c r="C22">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>62146</v>
+      </c>
+      <c r="C23">
+        <v>15536.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>472000</v>
+      </c>
+      <c r="C24">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>472000</v>
+      </c>
+      <c r="C25">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>113551</v>
+      </c>
+      <c r="C26">
+        <v>28387.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>78434</v>
+      </c>
+      <c r="C27">
+        <v>19608.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>472000</v>
+      </c>
+      <c r="C29">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>75336</v>
+      </c>
+      <c r="C30">
+        <v>18834</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>66886</v>
+      </c>
+      <c r="C31">
+        <v>16721.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>55553</v>
+      </c>
+      <c r="C32">
+        <v>13888.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>40771</v>
+      </c>
+      <c r="C33">
+        <v>10192.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>73907</v>
+      </c>
+      <c r="C34">
+        <v>18476.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>82043</v>
+      </c>
+      <c r="C35">
+        <v>20510.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>56903</v>
+      </c>
+      <c r="C36">
+        <v>14225.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>472000</v>
+      </c>
+      <c r="C37">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
         <v>72839</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
+      <c r="C38">
+        <v>18209.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>472000</v>
+      </c>
+      <c r="C39">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>51565</v>
+      </c>
+      <c r="C40">
+        <v>12891.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>82388</v>
+      </c>
+      <c r="C41">
+        <v>20597</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>472000</v>
+      </c>
+      <c r="C42">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>472000</v>
+      </c>
+      <c r="C43">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>472000</v>
+      </c>
+      <c r="C44">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>124114</v>
+      </c>
+      <c r="C45">
+        <v>31028.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>92734</v>
+      </c>
+      <c r="C46">
+        <v>23183.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>52423</v>
+      </c>
+      <c r="C47">
+        <v>13105.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>79915</v>
+      </c>
+      <c r="C48">
+        <v>19978.75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>472000</v>
+      </c>
+      <c r="C49">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
         <v>183598</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
+      <c r="C50">
+        <v>45899.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>23067</v>
+      </c>
+      <c r="C51">
+        <v>5766.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52">
+        <v>60325</v>
+      </c>
+      <c r="C52">
+        <v>15081.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53">
+        <v>52847</v>
+      </c>
+      <c r="C53">
+        <v>13211.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>128054</v>
+      </c>
+      <c r="C54">
+        <v>32013.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55">
         <v>52267</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
+      <c r="C55">
+        <v>13066.75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56">
+        <v>82580</v>
+      </c>
+      <c r="C56">
+        <v>20645</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57">
+        <v>472000</v>
+      </c>
+      <c r="C57">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>84528</v>
+      </c>
+      <c r="C58">
+        <v>21132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59">
+        <v>74660</v>
+      </c>
+      <c r="C59">
+        <v>18665</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <v>1736</v>
+      </c>
+      <c r="C60">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>56172</v>
+      </c>
+      <c r="C61">
+        <v>14043</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>472000</v>
+      </c>
+      <c r="C62">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63">
+        <v>119261</v>
+      </c>
+      <c r="C63">
+        <v>29815.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>170189</v>
+      </c>
+      <c r="C64">
+        <v>42547.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65">
+        <v>472000</v>
+      </c>
+      <c r="C65">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>47736</v>
+      </c>
+      <c r="C66">
+        <v>11934</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>15486</v>
+      </c>
+      <c r="C67">
+        <v>3871.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68">
         <v>82374</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
+      <c r="C68">
+        <v>20593.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <v>472000</v>
+      </c>
+      <c r="C69">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70">
+        <v>43355</v>
+      </c>
+      <c r="C70">
+        <v>10838.75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71">
+        <v>68062</v>
+      </c>
+      <c r="C71">
+        <v>17015.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>426613</v>
+      </c>
+      <c r="C72">
+        <v>106653.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>472000</v>
+      </c>
+      <c r="C73">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
         <v>70573</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
+      <c r="C74">
+        <v>17643.25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75">
+        <v>79126</v>
+      </c>
+      <c r="C75">
+        <v>19781.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76">
+        <v>1806</v>
+      </c>
+      <c r="C76">
+        <v>451.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77">
         <v>49127</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
+      <c r="C77">
+        <v>12281.75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>472000</v>
+      </c>
+      <c r="C78">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79">
+        <v>64629</v>
+      </c>
+      <c r="C79">
+        <v>16157.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80">
+        <v>472000</v>
+      </c>
+      <c r="C80">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81">
+        <v>88828</v>
+      </c>
+      <c r="C81">
+        <v>22207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82">
+        <v>83122</v>
+      </c>
+      <c r="C82">
+        <v>20780.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83">
+        <v>64212</v>
+      </c>
+      <c r="C83">
+        <v>16053</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84">
+        <v>152268</v>
+      </c>
+      <c r="C84">
+        <v>38067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85">
+        <v>78524</v>
+      </c>
+      <c r="C85">
+        <v>19631</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86">
+        <v>63783</v>
+      </c>
+      <c r="C86">
+        <v>15945.75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87">
+        <v>64269</v>
+      </c>
+      <c r="C87">
+        <v>16067.25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88">
+        <v>225848</v>
+      </c>
+      <c r="C88">
+        <v>56462</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89">
+        <v>472000</v>
+      </c>
+      <c r="C89">
+        <v>118000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90">
         <v>88878</v>
+      </c>
+      <c r="C90">
+        <v>22219.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91">
+        <v>53127</v>
+      </c>
+      <c r="C91">
+        <v>13281.75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92">
+        <v>36968</v>
+      </c>
+      <c r="C92">
+        <v>9242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>